<commit_message>
pushing to deploy to Netlify
</commit_message>
<xml_diff>
--- a/data/quiz_questions.xlsx
+++ b/data/quiz_questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\njlac\Documents\OSRS-Trivia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532450CD-FFB7-4ACE-BA8C-97C2C39BF92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A17641-9ED1-404A-B784-E24D25AFF4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EECF84FC-5D57-4091-8665-93435217BE69}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Question</t>
   </si>
@@ -92,13 +92,31 @@
     <t>Poop 2</t>
   </si>
   <si>
-    <t>Is Margaret the cutest?</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Yes</t>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>What crafting level is needed to spin a ball of wool?</t>
+  </si>
+  <si>
+    <t>What crafting level is needed to weave a drift net?</t>
+  </si>
+  <si>
+    <t>What quest must be completed before a player can wear a Green d'hide body?</t>
+  </si>
+  <si>
+    <t>Beneath Cursed Sands</t>
+  </si>
+  <si>
+    <t>One Small Favour</t>
+  </si>
+  <si>
+    <t>Tears of Guthix</t>
+  </si>
+  <si>
+    <t>What year was the Waterfall Quest initially released?</t>
+  </si>
+  <si>
+    <t>How many F2P quests are currently available?</t>
   </si>
 </sst>
 </file>
@@ -134,8 +152,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C5DE8B-CD85-43B9-9969-5FB249B22EDD}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,9 +503,10 @@
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -505,8 +525,11 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -525,8 +548,11 @@
       <c r="F2">
         <v>126</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -545,8 +571,11 @@
       <c r="F3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -565,8 +594,11 @@
       <c r="F4">
         <v>99</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -585,28 +617,127 @@
       <c r="F5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1">
+        <v>3.524</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>32</v>
+      </c>
+      <c r="D7">
+        <v>31</v>
+      </c>
+      <c r="E7">
+        <v>29</v>
+      </c>
+      <c r="F7">
+        <v>26</v>
+      </c>
+      <c r="G7" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4.26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>2002</v>
+      </c>
+      <c r="C9">
+        <v>2004</v>
+      </c>
+      <c r="D9">
+        <v>2001</v>
+      </c>
+      <c r="E9">
+        <v>2003</v>
+      </c>
+      <c r="F9">
+        <v>2002</v>
+      </c>
+      <c r="G9" s="1">
+        <v>5.67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>21</v>
+      </c>
+      <c r="D10">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
+      <c r="E10">
+        <v>24</v>
+      </c>
+      <c r="F10">
+        <v>22</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3.22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added change difficulty button
</commit_message>
<xml_diff>
--- a/data/quiz_questions.xlsx
+++ b/data/quiz_questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\njlac\Documents\OSRS-Trivia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A17641-9ED1-404A-B784-E24D25AFF4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FED5BBB-57D9-4FDE-9EE0-71E40650BFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EECF84FC-5D57-4091-8665-93435217BE69}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Question</t>
   </si>
@@ -117,6 +117,18 @@
   </si>
   <si>
     <t>How many F2P quests are currently available?</t>
+  </si>
+  <si>
+    <t>Is this the hardest question in the quiz?  9.99</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -489,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C5DE8B-CD85-43B9-9969-5FB249B22EDD}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +561,7 @@
         <v>126</v>
       </c>
       <c r="G2" s="1">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -572,7 +584,7 @@
         <v>8</v>
       </c>
       <c r="G3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -595,7 +607,7 @@
         <v>99</v>
       </c>
       <c r="G4" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -618,7 +630,7 @@
         <v>15</v>
       </c>
       <c r="G5" s="1">
-        <v>3.524</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -641,7 +653,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -664,7 +676,7 @@
         <v>26</v>
       </c>
       <c r="G7" s="1">
-        <v>7.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -687,7 +699,7 @@
         <v>9</v>
       </c>
       <c r="G8" s="1">
-        <v>4.26</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -710,7 +722,7 @@
         <v>2002</v>
       </c>
       <c r="G9" s="1">
-        <v>5.67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -733,7 +745,30 @@
         <v>22</v>
       </c>
       <c r="G10" s="1">
-        <v>3.22</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="1">
+        <v>9.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changing to difficulty choosing to be a range rather than one int
</commit_message>
<xml_diff>
--- a/data/quiz_questions.xlsx
+++ b/data/quiz_questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\njlac\Documents\OSRS-Trivia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FED5BBB-57D9-4FDE-9EE0-71E40650BFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57062C8-3926-404F-92DD-210015A5799C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EECF84FC-5D57-4091-8665-93435217BE69}"/>
   </bookViews>
@@ -504,7 +504,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>